<commit_message>
aggiornato es1 e update relazione es1
</commit_message>
<xml_diff>
--- a/relazioni/Grafici SRPT.xlsx
+++ b/relazioni/Grafici SRPT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessio/Desktop/Università/Simulazione e Performance/Forest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippo/Desktop/Network Simulation/Forest/relazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>utilizzo</t>
   </si>
@@ -52,12 +52,15 @@
   <si>
     <t>FIFO</t>
   </si>
+  <si>
+    <t>tps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +71,28 @@
     <font>
       <sz val="13"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,17 +115,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,6 +421,105 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$20:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.083519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.165702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.833185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.61647</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.6561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.0612</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.99687</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.994126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -395,56 +528,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539380560"/>
-        <c:axId val="539384672"/>
+        <c:axId val="89773056"/>
+        <c:axId val="192088336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539380560"/>
+        <c:axId val="89773056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT"/>
-                  <a:t>Lambda</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -511,12 +605,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539384672"/>
+        <c:crossAx val="192088336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539384672"/>
+        <c:axId val="192088336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -538,31 +632,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT"/>
-                  <a:t>% utilizzo</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -629,7 +698,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539380560"/>
+        <c:crossAx val="89773056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -641,6 +710,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -952,6 +1053,105 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$21:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.000836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.001657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.008332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.066165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.416562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91061</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.999967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.999941</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -960,30 +1160,72 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542331872"/>
-        <c:axId val="542334352"/>
+        <c:axId val="190289728"/>
+        <c:axId val="190291776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542331872"/>
+        <c:axId val="190289728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>LAMBDA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1021,12 +1263,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="542334352"/>
+        <c:crossAx val="190291776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542334352"/>
+        <c:axId val="190291776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1380,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="542331872"/>
+        <c:crossAx val="190289728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1150,6 +1392,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1303,10 +1577,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$M$3</c:f>
+              <c:f>Foglio1!$D$3:$O$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0E-6</c:v>
                 </c:pt>
@@ -1332,6 +1606,15 @@
                   <c:v>0.004</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
@@ -1339,10 +1622,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$D$6:$M$6</c:f>
+              <c:f>Foglio1!$D$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="#,##0">
                   <c:v>831.485</c:v>
                 </c:pt>
@@ -1367,7 +1650,7 @@
                 <c:pt idx="7">
                   <c:v>1284.439827</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>25276.67</c:v>
                 </c:pt>
               </c:numCache>
@@ -1408,10 +1691,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$M$3</c:f>
+              <c:f>Foglio1!$D$3:$O$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0E-6</c:v>
                 </c:pt>
@@ -1437,6 +1720,15 @@
                   <c:v>0.004</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
@@ -1444,10 +1736,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$D$7:$M$7</c:f>
+              <c:f>Foglio1!$D$7:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.036069</c:v>
                 </c:pt>
@@ -1472,7 +1764,7 @@
                 <c:pt idx="7">
                   <c:v>703.20969</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>25212.67</c:v>
                 </c:pt>
               </c:numCache>
@@ -1488,11 +1780,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="542360048"/>
-        <c:axId val="542363808"/>
+        <c:axId val="190316384"/>
+        <c:axId val="190320144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="542360048"/>
+        <c:axId val="190316384"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1605,12 +1897,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="542363808"/>
+        <c:crossAx val="190320144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="542363808"/>
+        <c:axId val="190320144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,7 +2014,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="542360048"/>
+        <c:crossAx val="190316384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2184,11 +2476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539420208"/>
-        <c:axId val="539423968"/>
+        <c:axId val="190335856"/>
+        <c:axId val="190339200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539420208"/>
+        <c:axId val="190335856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2301,12 +2593,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539423968"/>
+        <c:crossAx val="190339200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539423968"/>
+        <c:axId val="190339200"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2420,7 +2712,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539420208"/>
+        <c:crossAx val="190335856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2794,11 +3086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539455488"/>
-        <c:axId val="539459984"/>
+        <c:axId val="192119792"/>
+        <c:axId val="190365744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539455488"/>
+        <c:axId val="192119792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,12 +3178,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539459984"/>
+        <c:crossAx val="190365744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539459984"/>
+        <c:axId val="190365744"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2979,7 +3271,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539455488"/>
+        <c:crossAx val="192119792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3345,7 +3637,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3353,11 +3644,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="573489456"/>
-        <c:axId val="573340064"/>
+        <c:axId val="190373008"/>
+        <c:axId val="190376352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="573489456"/>
+        <c:axId val="190373008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3444,12 +3735,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573340064"/>
+        <c:crossAx val="190376352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="573340064"/>
+        <c:axId val="190376352"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3538,7 +3829,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573489456"/>
+        <c:crossAx val="190373008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3552,6 +3843,706 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Throughput all'aumentare di Lambda</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SRPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.001102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.001354</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.001729</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.002861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RANDOM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$11:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$17:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.001105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.001203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.001208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$25:$L$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.001101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.001202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.001199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.001208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="266042384"/>
+        <c:axId val="260678512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="266042384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>LAMBDA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="260678512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="260678512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Throughput</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266042384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3859,6 +4850,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -6979,20 +8010,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>819851</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1407</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>14112</xdr:rowOff>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
+      <xdr:colOff>522110</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>42334</xdr:rowOff>
+      <xdr:rowOff>112889</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7014,15 +8565,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>14110</xdr:colOff>
+      <xdr:colOff>28221</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>14111</xdr:rowOff>
+      <xdr:rowOff>84666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>395109</xdr:colOff>
+      <xdr:colOff>409220</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>70555</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7163,6 +8714,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>380998</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>14111</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Grafico 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7429,10 +9012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:M24"/>
+  <dimension ref="C3:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7442,7 +9025,7 @@
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -7471,10 +9054,19 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L3">
+        <v>0.01</v>
+      </c>
+      <c r="M3">
+        <v>0.03</v>
+      </c>
+      <c r="N3">
+        <v>0.1</v>
+      </c>
+      <c r="O3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="3:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -7502,11 +9094,11 @@
       <c r="K4">
         <v>99.998456000000004</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>99.983975000000001</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -7534,11 +9126,11 @@
       <c r="K5">
         <v>0.99998399999999998</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>0.99975000000000003</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:15" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -7566,12 +9158,11 @@
       <c r="K6" s="3">
         <v>1284.4398269999999</v>
       </c>
-      <c r="L6" s="3">
+      <c r="O6" s="3">
         <v>25276.67</v>
       </c>
-      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -7599,12 +9190,11 @@
       <c r="K7">
         <v>703.20969000000002</v>
       </c>
-      <c r="L7" s="3">
+      <c r="O7" s="3">
         <v>25212.67</v>
       </c>
-      <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -7632,12 +9222,49 @@
       <c r="K8">
         <v>79272</v>
       </c>
-      <c r="L8" s="3">
+      <c r="O8" s="3">
         <v>17669</v>
       </c>
-      <c r="M8" s="3"/>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E9">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G9">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H9">
+        <v>4.9899999999999999E-4</v>
+      </c>
+      <c r="I9">
+        <v>1.1019999999999999E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.354E-3</v>
+      </c>
+      <c r="K9">
+        <v>1.7290000000000001E-3</v>
+      </c>
+      <c r="L9">
+        <v>2.8609999999999998E-3</v>
+      </c>
+      <c r="M9">
+        <v>6.587E-3</v>
+      </c>
+      <c r="N9">
+        <v>1.5624000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -7665,8 +9292,17 @@
       <c r="K11">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="L11">
+        <v>0.01</v>
+      </c>
+      <c r="M11">
+        <v>0.03</v>
+      </c>
+      <c r="N11">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -7695,7 +9331,7 @@
         <v>99.999835000000004</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>1</v>
       </c>
@@ -7724,7 +9360,7 @@
         <v>0.99999979999999999</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>2</v>
       </c>
@@ -7753,7 +9389,7 @@
         <v>7913445.71</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -7782,7 +9418,7 @@
         <v>7912613.6740629999</v>
       </c>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -7811,7 +9447,45 @@
         <v>107691</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E17">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F17">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G17">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5.0299999999999997E-4</v>
+      </c>
+      <c r="I17">
+        <v>1.1050000000000001E-3</v>
+      </c>
+      <c r="J17">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K17">
+        <v>1.2030000000000001E-3</v>
+      </c>
+      <c r="L17">
+        <v>1.2080000000000001E-3</v>
+      </c>
+      <c r="M17">
+        <v>1.2099999999999999E-3</v>
+      </c>
+      <c r="N17">
+        <v>1.196E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>7</v>
       </c>
@@ -7839,8 +9513,17 @@
       <c r="K19">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="L19">
+        <v>0.01</v>
+      </c>
+      <c r="M19">
+        <v>0.03</v>
+      </c>
+      <c r="N19">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -7869,7 +9552,7 @@
         <v>99.994125999999994</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>1</v>
       </c>
@@ -7898,7 +9581,7 @@
         <v>0.99994099999999997</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -7927,7 +9610,7 @@
         <v>13436458</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>3</v>
       </c>
@@ -7956,7 +9639,7 @@
         <v>13435628</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>4</v>
       </c>
@@ -7983,6 +9666,44 @@
       </c>
       <c r="K24" s="4">
         <v>107356</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E25">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G25">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>5.0100000000000003E-4</v>
+      </c>
+      <c r="I25">
+        <v>1.101E-3</v>
+      </c>
+      <c r="J25">
+        <v>1.2019999999999999E-3</v>
+      </c>
+      <c r="K25">
+        <v>1.199E-3</v>
+      </c>
+      <c r="L25">
+        <v>1.2080000000000001E-3</v>
+      </c>
+      <c r="M25">
+        <v>1.2099999999999999E-3</v>
+      </c>
+      <c r="N25">
+        <v>1.2099999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>